<commit_message>
Date Calculations (NOW, TODAY, YEARFRAC), Final Assessment
</commit_message>
<xml_diff>
--- a/Intermediate I/Week 2/workbook/W2_V5 Date_Functions.xlsx
+++ b/Intermediate I/Week 2/workbook/W2_V5 Date_Functions.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users-Data\mq20021873\Desktop\Coursera 20 April 2017\Course 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\foongmin\Desktop\excel-skills-for-business\Intermediate I\Week 2\workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59714FC2-79F8-4B3F-B95D-154E690698F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9672"/>
+    <workbookView xWindow="10330" yWindow="50" windowWidth="9620" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,10 +18,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$J$24</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -512,7 +521,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -933,40 +942,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4:N38"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:I38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.21875" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" customWidth="1"/>
     <col min="2" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="30.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.90625" customWidth="1"/>
+    <col min="5" max="5" width="30.08984375" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" customWidth="1"/>
-    <col min="13" max="13" width="12.77734375" customWidth="1"/>
-    <col min="14" max="14" width="16.109375" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" customWidth="1"/>
+    <col min="8" max="9" width="13.6328125" customWidth="1"/>
+    <col min="10" max="10" width="17.6328125" customWidth="1"/>
+    <col min="11" max="11" width="16.08984375" customWidth="1"/>
+    <col min="12" max="12" width="10.453125" customWidth="1"/>
+    <col min="13" max="13" width="12.81640625" customWidth="1"/>
+    <col min="14" max="14" width="16.08984375" customWidth="1"/>
+    <col min="15" max="15" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
         <v>117</v>
       </c>
       <c r="M1" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="N1" s="8"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N1" s="8">
+        <f ca="1">NOW()</f>
+        <v>43997.493437731478</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1010,7 +1022,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -1031,11 +1043,17 @@
       <c r="F4" s="1">
         <v>39556</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3">
+        <f ca="1">YEARFRAC(F4,TODAY())</f>
+        <v>12.158333333333333</v>
+      </c>
       <c r="H4" s="1">
         <v>42552</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="I4" s="1">
+        <f>H4+365</f>
+        <v>42917</v>
+      </c>
       <c r="J4" s="2" t="s">
         <v>72</v>
       </c>
@@ -1059,7 +1077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -1080,11 +1098,17 @@
       <c r="F5" s="1">
         <v>38104</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="3">
+        <f t="shared" ref="G5:G38" ca="1" si="2">YEARFRAC(F5,TODAY())</f>
+        <v>16.133333333333333</v>
+      </c>
       <c r="H5" s="1">
         <v>42825</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="I5" s="1">
+        <f t="shared" ref="I5:I38" si="3">H5+365</f>
+        <v>43190</v>
+      </c>
       <c r="J5" s="2" t="s">
         <v>36</v>
       </c>
@@ -1092,23 +1116,23 @@
         <v>120</v>
       </c>
       <c r="L5" s="1" t="str">
-        <f t="shared" ref="L5:L38" si="2">LEFT(K5,2)</f>
+        <f t="shared" ref="L5:L38" si="4">LEFT(K5,2)</f>
         <v>02</v>
       </c>
       <c r="M5" s="5" t="str">
-        <f t="shared" ref="M5:M38" si="3">RIGHT(K5,4)</f>
+        <f t="shared" ref="M5:M38" si="5">RIGHT(K5,4)</f>
         <v>2018</v>
       </c>
       <c r="N5" t="str">
-        <f t="shared" ref="N5:N38" si="4">MID(K5,4,FIND(" ",K5)-4)</f>
+        <f t="shared" ref="N5:N38" si="6">MID(K5,4,FIND(" ",K5)-4)</f>
         <v>West</v>
       </c>
       <c r="O5">
-        <f t="shared" ref="O5:O38" si="5">FIND(" ",K5)-4</f>
+        <f t="shared" ref="O5:O38" si="7">FIND(" ",K5)-4</f>
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -1129,11 +1153,17 @@
       <c r="F6" s="1">
         <v>41961</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.5750000000000002</v>
+      </c>
       <c r="H6" s="1">
         <v>42656</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="I6" s="1">
+        <f t="shared" si="3"/>
+        <v>43021</v>
+      </c>
       <c r="J6" s="2" t="s">
         <v>72</v>
       </c>
@@ -1141,23 +1171,23 @@
         <v>121</v>
       </c>
       <c r="L6" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>02</v>
       </c>
       <c r="M6" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2347</v>
       </c>
       <c r="N6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>West</v>
       </c>
       <c r="O6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>108</v>
       </c>
@@ -1178,11 +1208,17 @@
       <c r="F7" s="1">
         <v>42234</v>
       </c>
-      <c r="G7" s="3"/>
+      <c r="G7" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.8250000000000002</v>
+      </c>
       <c r="H7" s="1">
         <v>42804</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1">
+        <f t="shared" si="3"/>
+        <v>43169</v>
+      </c>
       <c r="J7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1190,23 +1226,23 @@
         <v>122</v>
       </c>
       <c r="L7" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>03</v>
       </c>
       <c r="M7" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2764</v>
       </c>
       <c r="N7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>West</v>
       </c>
       <c r="O7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>112</v>
       </c>
@@ -1227,11 +1263,17 @@
       <c r="F8" s="1">
         <v>42389</v>
       </c>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.4027777777777777</v>
+      </c>
       <c r="H8" s="1">
         <v>42566</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="1">
+        <f t="shared" si="3"/>
+        <v>42931</v>
+      </c>
       <c r="J8" s="2" t="s">
         <v>72</v>
       </c>
@@ -1239,23 +1281,23 @@
         <v>123</v>
       </c>
       <c r="L8" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>02</v>
       </c>
       <c r="M8" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2589</v>
       </c>
       <c r="N8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>West</v>
       </c>
       <c r="O8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -1276,11 +1318,17 @@
       <c r="F9" s="1">
         <v>41898</v>
       </c>
-      <c r="G9" s="3"/>
+      <c r="G9" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.7472222222222218</v>
+      </c>
       <c r="H9" s="1">
         <v>42551</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="I9" s="1">
+        <f t="shared" si="3"/>
+        <v>42916</v>
+      </c>
       <c r="J9" s="2" t="s">
         <v>21</v>
       </c>
@@ -1288,23 +1336,23 @@
         <v>139</v>
       </c>
       <c r="L9" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>03</v>
       </c>
       <c r="M9" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2318</v>
       </c>
       <c r="N9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>North</v>
       </c>
       <c r="O9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>102</v>
       </c>
@@ -1325,11 +1373,17 @@
       <c r="F10" s="1">
         <v>41908</v>
       </c>
-      <c r="G10" s="3"/>
+      <c r="G10" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.7194444444444441</v>
+      </c>
       <c r="H10" s="1">
         <v>42619</v>
       </c>
-      <c r="I10" s="1"/>
+      <c r="I10" s="1">
+        <f t="shared" si="3"/>
+        <v>42984</v>
+      </c>
       <c r="J10" s="2" t="s">
         <v>72</v>
       </c>
@@ -1337,23 +1391,23 @@
         <v>140</v>
       </c>
       <c r="L10" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>02</v>
       </c>
       <c r="M10" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2694</v>
       </c>
       <c r="N10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>North</v>
       </c>
       <c r="O10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>88</v>
       </c>
@@ -1374,11 +1428,17 @@
       <c r="F11" s="1">
         <v>38803</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>14.216666666666667</v>
+      </c>
       <c r="H11" s="1">
         <v>42761</v>
       </c>
-      <c r="I11" s="1"/>
+      <c r="I11" s="1">
+        <f t="shared" si="3"/>
+        <v>43126</v>
+      </c>
       <c r="J11" s="2" t="s">
         <v>72</v>
       </c>
@@ -1386,23 +1446,23 @@
         <v>124</v>
       </c>
       <c r="L11" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>02</v>
       </c>
       <c r="M11" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2699</v>
       </c>
       <c r="N11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>West</v>
       </c>
       <c r="O11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1423,11 +1483,17 @@
       <c r="F12" s="1">
         <v>36928</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>19.358333333333334</v>
+      </c>
       <c r="H12" s="1">
         <v>42596</v>
       </c>
-      <c r="I12" s="1"/>
+      <c r="I12" s="1">
+        <f t="shared" si="3"/>
+        <v>42961</v>
+      </c>
       <c r="J12" s="2" t="s">
         <v>34</v>
       </c>
@@ -1435,23 +1501,23 @@
         <v>141</v>
       </c>
       <c r="L12" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>01</v>
       </c>
       <c r="M12" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2321</v>
       </c>
       <c r="N12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>North</v>
       </c>
       <c r="O12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>100</v>
       </c>
@@ -1472,11 +1538,17 @@
       <c r="F13" s="1">
         <v>41792</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.0361111111111114</v>
+      </c>
       <c r="H13" s="1">
         <v>42544</v>
       </c>
-      <c r="I13" s="1"/>
+      <c r="I13" s="1">
+        <f t="shared" si="3"/>
+        <v>42909</v>
+      </c>
       <c r="J13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1484,23 +1556,23 @@
         <v>125</v>
       </c>
       <c r="L13" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>03</v>
       </c>
       <c r="M13" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2432</v>
       </c>
       <c r="N13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>West</v>
       </c>
       <c r="O13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -1521,11 +1593,17 @@
       <c r="F14" s="1">
         <v>40595</v>
       </c>
-      <c r="G14" s="3"/>
+      <c r="G14" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>9.3166666666666664</v>
+      </c>
       <c r="H14" s="1">
         <v>42629</v>
       </c>
-      <c r="I14" s="1"/>
+      <c r="I14" s="1">
+        <f t="shared" si="3"/>
+        <v>42994</v>
+      </c>
       <c r="J14" s="2" t="s">
         <v>72</v>
       </c>
@@ -1533,23 +1611,23 @@
         <v>126</v>
       </c>
       <c r="L14" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>02</v>
       </c>
       <c r="M14" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2962</v>
       </c>
       <c r="N14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>West</v>
       </c>
       <c r="O14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>96</v>
       </c>
@@ -1570,11 +1648,17 @@
       <c r="F15" s="1">
         <v>40994</v>
       </c>
-      <c r="G15" s="3"/>
+      <c r="G15" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>8.219444444444445</v>
+      </c>
       <c r="H15" s="1">
         <v>42848</v>
       </c>
-      <c r="I15" s="1"/>
+      <c r="I15" s="1">
+        <f t="shared" si="3"/>
+        <v>43213</v>
+      </c>
       <c r="J15" s="2" t="s">
         <v>23</v>
       </c>
@@ -1582,23 +1666,23 @@
         <v>142</v>
       </c>
       <c r="L15" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>03</v>
       </c>
       <c r="M15" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2134</v>
       </c>
       <c r="N15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>North</v>
       </c>
       <c r="O15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>93</v>
       </c>
@@ -1619,11 +1703,17 @@
       <c r="F16" s="1">
         <v>40225</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>10.330555555555556</v>
+      </c>
       <c r="H16" s="1">
         <v>42860</v>
       </c>
-      <c r="I16" s="1"/>
+      <c r="I16" s="1">
+        <f t="shared" si="3"/>
+        <v>43225</v>
+      </c>
       <c r="J16" s="2" t="s">
         <v>80</v>
       </c>
@@ -1631,23 +1721,23 @@
         <v>127</v>
       </c>
       <c r="L16" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>01</v>
       </c>
       <c r="M16" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2425</v>
       </c>
       <c r="N16" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>West</v>
       </c>
       <c r="O16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1668,11 +1758,17 @@
       <c r="F17" s="1">
         <v>36955</v>
       </c>
-      <c r="G17" s="3"/>
+      <c r="G17" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>19.277777777777779</v>
+      </c>
       <c r="H17" s="1">
         <v>42540</v>
       </c>
-      <c r="I17" s="1"/>
+      <c r="I17" s="1">
+        <f t="shared" si="3"/>
+        <v>42905</v>
+      </c>
       <c r="J17" s="2" t="s">
         <v>80</v>
       </c>
@@ -1680,23 +1776,23 @@
         <v>128</v>
       </c>
       <c r="L17" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>03</v>
       </c>
       <c r="M17" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2796</v>
       </c>
       <c r="N17" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>West</v>
       </c>
       <c r="O17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>116</v>
       </c>
@@ -1717,11 +1813,17 @@
       <c r="F18" s="1">
         <v>42912</v>
       </c>
-      <c r="G18" s="3"/>
+      <c r="G18" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>2.9694444444444446</v>
+      </c>
       <c r="H18" s="1">
         <v>42828</v>
       </c>
-      <c r="I18" s="1"/>
+      <c r="I18" s="1">
+        <f t="shared" si="3"/>
+        <v>43193</v>
+      </c>
       <c r="J18" s="2" t="s">
         <v>36</v>
       </c>
@@ -1729,23 +1831,23 @@
         <v>130</v>
       </c>
       <c r="L18" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>02</v>
       </c>
       <c r="M18" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2414</v>
       </c>
       <c r="N18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>West</v>
       </c>
       <c r="O18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>104</v>
       </c>
@@ -1766,11 +1868,17 @@
       <c r="F19" s="1">
         <v>41995</v>
       </c>
-      <c r="G19" s="3"/>
+      <c r="G19" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.4805555555555552</v>
+      </c>
       <c r="H19" s="1">
         <v>42731</v>
       </c>
-      <c r="I19" s="1"/>
+      <c r="I19" s="1">
+        <f t="shared" si="3"/>
+        <v>43096</v>
+      </c>
       <c r="J19" s="2" t="s">
         <v>21</v>
       </c>
@@ -1778,23 +1886,23 @@
         <v>129</v>
       </c>
       <c r="L19" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>03</v>
       </c>
       <c r="M19" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2601</v>
       </c>
       <c r="N19" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>West</v>
       </c>
       <c r="O19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -1815,11 +1923,17 @@
       <c r="F20" s="1">
         <v>41407</v>
       </c>
-      <c r="G20" s="3"/>
+      <c r="G20" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.0888888888888886</v>
+      </c>
       <c r="H20" s="1">
         <v>42720</v>
       </c>
-      <c r="I20" s="1"/>
+      <c r="I20" s="1">
+        <f t="shared" si="3"/>
+        <v>43085</v>
+      </c>
       <c r="J20" s="2" t="s">
         <v>36</v>
       </c>
@@ -1827,23 +1941,23 @@
         <v>131</v>
       </c>
       <c r="L20" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>02</v>
       </c>
       <c r="M20" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2537</v>
       </c>
       <c r="N20" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>West</v>
       </c>
       <c r="O20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>91</v>
       </c>
@@ -1864,11 +1978,17 @@
       <c r="F21" s="1">
         <v>39692</v>
       </c>
-      <c r="G21" s="3"/>
+      <c r="G21" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>11.78888888888889</v>
+      </c>
       <c r="H21" s="1">
         <v>42598</v>
       </c>
-      <c r="I21" s="1"/>
+      <c r="I21" s="1">
+        <f t="shared" si="3"/>
+        <v>42963</v>
+      </c>
       <c r="J21" s="2" t="s">
         <v>36</v>
       </c>
@@ -1876,23 +1996,23 @@
         <v>132</v>
       </c>
       <c r="L21" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>02</v>
       </c>
       <c r="M21" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2286</v>
       </c>
       <c r="N21" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>West</v>
       </c>
       <c r="O21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>98</v>
       </c>
@@ -1913,11 +2033,17 @@
       <c r="F22" s="1">
         <v>41214</v>
       </c>
-      <c r="G22" s="3"/>
+      <c r="G22" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.6222222222222218</v>
+      </c>
       <c r="H22" s="1">
         <v>42566</v>
       </c>
-      <c r="I22" s="1"/>
+      <c r="I22" s="1">
+        <f t="shared" si="3"/>
+        <v>42931</v>
+      </c>
       <c r="J22" s="2" t="s">
         <v>80</v>
       </c>
@@ -1925,23 +2051,23 @@
         <v>143</v>
       </c>
       <c r="L22" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>01</v>
       </c>
       <c r="M22" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2086</v>
       </c>
       <c r="N22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>North</v>
       </c>
       <c r="O22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -1962,11 +2088,17 @@
       <c r="F23" s="1">
         <v>41176</v>
       </c>
-      <c r="G23" s="3"/>
+      <c r="G23" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>7.7249999999999996</v>
+      </c>
       <c r="H23" s="1">
         <v>42835</v>
       </c>
-      <c r="I23" s="1"/>
+      <c r="I23" s="1">
+        <f t="shared" si="3"/>
+        <v>43200</v>
+      </c>
       <c r="J23" t="s">
         <v>80</v>
       </c>
@@ -1974,23 +2106,23 @@
         <v>144</v>
       </c>
       <c r="L23" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>01</v>
       </c>
       <c r="M23" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2358</v>
       </c>
       <c r="N23" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>North</v>
       </c>
       <c r="O23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>107</v>
       </c>
@@ -2011,11 +2143,17 @@
       <c r="F24" s="1">
         <v>42233</v>
       </c>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.8277777777777775</v>
+      </c>
       <c r="H24" s="1">
         <v>42658</v>
       </c>
-      <c r="I24" s="1"/>
+      <c r="I24" s="1">
+        <f t="shared" si="3"/>
+        <v>43023</v>
+      </c>
       <c r="J24" s="2" t="s">
         <v>21</v>
       </c>
@@ -2023,23 +2161,23 @@
         <v>133</v>
       </c>
       <c r="L24" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>03</v>
       </c>
       <c r="M24" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2082</v>
       </c>
       <c r="N24" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>West</v>
       </c>
       <c r="O24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>111</v>
       </c>
@@ -2060,11 +2198,17 @@
       <c r="F25" s="1">
         <v>42376</v>
       </c>
-      <c r="G25" s="3"/>
+      <c r="G25" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.4388888888888891</v>
+      </c>
       <c r="H25" s="1">
         <v>42614</v>
       </c>
-      <c r="I25" s="1"/>
+      <c r="I25" s="1">
+        <f t="shared" si="3"/>
+        <v>42979</v>
+      </c>
       <c r="J25" s="2" t="s">
         <v>80</v>
       </c>
@@ -2072,23 +2216,23 @@
         <v>134</v>
       </c>
       <c r="L25" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>03</v>
       </c>
       <c r="M25" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2482</v>
       </c>
       <c r="N25" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>West</v>
       </c>
       <c r="O25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>89</v>
       </c>
@@ -2109,11 +2253,17 @@
       <c r="F26" s="1">
         <v>39028</v>
       </c>
-      <c r="G26" s="3"/>
+      <c r="G26" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>13.605555555555556</v>
+      </c>
       <c r="H26" s="1">
         <v>42817</v>
       </c>
-      <c r="I26" s="1"/>
+      <c r="I26" s="1">
+        <f t="shared" si="3"/>
+        <v>43182</v>
+      </c>
       <c r="J26" s="2" t="s">
         <v>21</v>
       </c>
@@ -2121,23 +2271,23 @@
         <v>145</v>
       </c>
       <c r="L26" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>02</v>
       </c>
       <c r="M26" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2372</v>
       </c>
       <c r="N26" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>North</v>
       </c>
       <c r="O26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -2158,11 +2308,17 @@
       <c r="F27" s="1">
         <v>38553</v>
       </c>
-      <c r="G27" s="3"/>
+      <c r="G27" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>14.902777777777779</v>
+      </c>
       <c r="H27" s="1">
         <v>42845</v>
       </c>
-      <c r="I27" s="1"/>
+      <c r="I27" s="1">
+        <f t="shared" si="3"/>
+        <v>43210</v>
+      </c>
       <c r="J27" s="2" t="s">
         <v>72</v>
       </c>
@@ -2170,23 +2326,23 @@
         <v>146</v>
       </c>
       <c r="L27" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>03</v>
       </c>
       <c r="M27" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2392</v>
       </c>
       <c r="N27" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>North</v>
       </c>
       <c r="O27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -2207,11 +2363,17 @@
       <c r="F28" s="1">
         <v>38749</v>
       </c>
-      <c r="G28" s="3"/>
+      <c r="G28" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>14.372222222222222</v>
+      </c>
       <c r="H28" s="1">
         <v>42776</v>
       </c>
-      <c r="I28" s="1"/>
+      <c r="I28" s="1">
+        <f t="shared" si="3"/>
+        <v>43141</v>
+      </c>
       <c r="J28" s="2" t="s">
         <v>36</v>
       </c>
@@ -2219,23 +2381,23 @@
         <v>135</v>
       </c>
       <c r="L28" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>02</v>
       </c>
       <c r="M28" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2279</v>
       </c>
       <c r="N28" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>West</v>
       </c>
       <c r="O28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -2256,11 +2418,17 @@
       <c r="F29" s="1">
         <v>37515</v>
       </c>
-      <c r="G29" s="3"/>
+      <c r="G29" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>17.747222222222224</v>
+      </c>
       <c r="H29" s="1">
         <v>42586</v>
       </c>
-      <c r="I29" s="1"/>
+      <c r="I29" s="1">
+        <f t="shared" si="3"/>
+        <v>42951</v>
+      </c>
       <c r="J29" s="2" t="s">
         <v>72</v>
       </c>
@@ -2268,23 +2436,23 @@
         <v>147</v>
       </c>
       <c r="L29" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>02</v>
       </c>
       <c r="M29" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2639</v>
       </c>
       <c r="N29" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>North</v>
       </c>
       <c r="O29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>106</v>
       </c>
@@ -2305,11 +2473,17 @@
       <c r="F30" s="1">
         <v>42125</v>
       </c>
-      <c r="G30" s="3"/>
+      <c r="G30" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.1222222222222218</v>
+      </c>
       <c r="H30" s="1">
         <v>42710</v>
       </c>
-      <c r="I30" s="1"/>
+      <c r="I30" s="1">
+        <f t="shared" si="3"/>
+        <v>43075</v>
+      </c>
       <c r="J30" s="2" t="s">
         <v>72</v>
       </c>
@@ -2317,23 +2491,23 @@
         <v>148</v>
       </c>
       <c r="L30" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>02</v>
       </c>
       <c r="M30" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2284</v>
       </c>
       <c r="N30" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>North</v>
       </c>
       <c r="O30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -2354,11 +2528,17 @@
       <c r="F31" s="1">
         <v>42726</v>
       </c>
-      <c r="G31" s="3"/>
+      <c r="G31" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>3.4805555555555556</v>
+      </c>
       <c r="H31" s="1">
         <v>42539</v>
       </c>
-      <c r="I31" s="1"/>
+      <c r="I31" s="1">
+        <f t="shared" si="3"/>
+        <v>42904</v>
+      </c>
       <c r="J31" s="2" t="s">
         <v>72</v>
       </c>
@@ -2366,23 +2546,23 @@
         <v>149</v>
       </c>
       <c r="L31" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>02</v>
       </c>
       <c r="M31" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2910</v>
       </c>
       <c r="N31" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>North</v>
       </c>
       <c r="O31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>92</v>
       </c>
@@ -2403,11 +2583,17 @@
       <c r="F32" s="1">
         <v>40162</v>
       </c>
-      <c r="G32" s="3"/>
+      <c r="G32" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>10.5</v>
+      </c>
       <c r="H32" s="1">
         <v>42563</v>
       </c>
-      <c r="I32" s="1"/>
+      <c r="I32" s="1">
+        <f t="shared" si="3"/>
+        <v>42928</v>
+      </c>
       <c r="J32" s="2" t="s">
         <v>72</v>
       </c>
@@ -2415,23 +2601,23 @@
         <v>150</v>
       </c>
       <c r="L32" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>02</v>
       </c>
       <c r="M32" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2294</v>
       </c>
       <c r="N32" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>North</v>
       </c>
       <c r="O32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>113</v>
       </c>
@@ -2452,11 +2638,17 @@
       <c r="F33" s="1">
         <v>42892</v>
       </c>
-      <c r="G33" s="3"/>
+      <c r="G33" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>3.0249999999999999</v>
+      </c>
       <c r="H33" s="1">
         <v>42731</v>
       </c>
-      <c r="I33" s="1"/>
+      <c r="I33" s="1">
+        <f t="shared" si="3"/>
+        <v>43096</v>
+      </c>
       <c r="J33" s="2" t="s">
         <v>23</v>
       </c>
@@ -2464,23 +2656,23 @@
         <v>136</v>
       </c>
       <c r="L33" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>03</v>
       </c>
       <c r="M33" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2765</v>
       </c>
       <c r="N33" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>West</v>
       </c>
       <c r="O33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>110</v>
       </c>
@@ -2501,11 +2693,17 @@
       <c r="F34" s="1">
         <v>42325</v>
       </c>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.5777777777777775</v>
+      </c>
       <c r="H34" s="1">
         <v>42590</v>
       </c>
-      <c r="I34" s="1"/>
+      <c r="I34" s="1">
+        <f t="shared" si="3"/>
+        <v>42955</v>
+      </c>
       <c r="J34" s="2" t="s">
         <v>72</v>
       </c>
@@ -2513,23 +2711,23 @@
         <v>151</v>
       </c>
       <c r="L34" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>02</v>
       </c>
       <c r="M34" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2260</v>
       </c>
       <c r="N34" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>North</v>
       </c>
       <c r="O34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>95</v>
       </c>
@@ -2550,11 +2748,17 @@
       <c r="F35" s="1">
         <v>40714</v>
       </c>
-      <c r="G35" s="3"/>
+      <c r="G35" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>8.9861111111111107</v>
+      </c>
       <c r="H35" s="1">
         <v>42507</v>
       </c>
-      <c r="I35" s="1"/>
+      <c r="I35" s="1">
+        <f t="shared" si="3"/>
+        <v>42872</v>
+      </c>
       <c r="J35" s="2" t="s">
         <v>72</v>
       </c>
@@ -2562,23 +2766,23 @@
         <v>156</v>
       </c>
       <c r="L35" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>02</v>
       </c>
       <c r="M35" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2578</v>
       </c>
       <c r="N35" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>West</v>
       </c>
       <c r="O35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>109</v>
       </c>
@@ -2599,11 +2803,17 @@
       <c r="F36" s="1">
         <v>42326</v>
       </c>
-      <c r="G36" s="3"/>
+      <c r="G36" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.5750000000000002</v>
+      </c>
       <c r="H36" s="1">
         <v>42801</v>
       </c>
-      <c r="I36" s="1"/>
+      <c r="I36" s="1">
+        <f t="shared" si="3"/>
+        <v>43166</v>
+      </c>
       <c r="J36" s="2" t="s">
         <v>72</v>
       </c>
@@ -2611,23 +2821,23 @@
         <v>152</v>
       </c>
       <c r="L36" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>02</v>
       </c>
       <c r="M36" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2654</v>
       </c>
       <c r="N36" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>North</v>
       </c>
       <c r="O36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>115</v>
       </c>
@@ -2648,11 +2858,17 @@
       <c r="F37" s="1">
         <v>40189</v>
       </c>
-      <c r="G37" s="3"/>
+      <c r="G37" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>10.427777777777777</v>
+      </c>
       <c r="H37" s="1">
         <v>42839</v>
       </c>
-      <c r="I37" s="1"/>
+      <c r="I37" s="1">
+        <f t="shared" si="3"/>
+        <v>43204</v>
+      </c>
       <c r="J37" s="2" t="s">
         <v>34</v>
       </c>
@@ -2660,23 +2876,23 @@
         <v>137</v>
       </c>
       <c r="L37" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>01</v>
       </c>
       <c r="M37" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2783</v>
       </c>
       <c r="N37" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>West</v>
       </c>
       <c r="O37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>105</v>
       </c>
@@ -2697,11 +2913,17 @@
       <c r="F38" s="1">
         <v>42009</v>
       </c>
-      <c r="G38" s="3"/>
+      <c r="G38" s="3">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.4444444444444446</v>
+      </c>
       <c r="H38" s="1">
         <v>42652</v>
       </c>
-      <c r="I38" s="1"/>
+      <c r="I38" s="1">
+        <f t="shared" si="3"/>
+        <v>43017</v>
+      </c>
       <c r="J38" s="2" t="s">
         <v>72</v>
       </c>
@@ -2709,24 +2931,24 @@
         <v>153</v>
       </c>
       <c r="L38" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>02</v>
       </c>
       <c r="M38" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2793</v>
       </c>
       <c r="N38" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>North</v>
       </c>
       <c r="O38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:M38">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:M38">
     <sortCondition ref="B6"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>